<commit_message>
Add Stata versions of tables for compiling results.
</commit_message>
<xml_diff>
--- a/Tables/t1_balance.xlsx
+++ b/Tables/t1_balance.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="144">
   <si>
     <t>Factor</t>
   </si>
@@ -363,9 +363,6 @@
     <t>9564.00 (10541.79)</t>
   </si>
   <si>
-    <t>3.86</t>
-  </si>
-  <si>
     <t>p-value</t>
   </si>
   <si>
@@ -448,9 +445,6 @@
   </si>
   <si>
     <t>0.20</t>
-  </si>
-  <si>
-    <t>0.356</t>
   </si>
 </sst>
 </file>
@@ -508,7 +502,7 @@
         <v>80</v>
       </c>
       <c r="D1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2">
@@ -536,7 +530,7 @@
         <v>82</v>
       </c>
       <c r="D3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4">
@@ -550,7 +544,7 @@
         <v>83</v>
       </c>
       <c r="D4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5">
@@ -564,7 +558,7 @@
         <v>46</v>
       </c>
       <c r="D5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6">
@@ -620,7 +614,7 @@
         <v>87</v>
       </c>
       <c r="D9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10">
@@ -634,7 +628,7 @@
         <v>88</v>
       </c>
       <c r="D10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11">
@@ -648,7 +642,7 @@
         <v>89</v>
       </c>
       <c r="D11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="12">
@@ -662,7 +656,7 @@
         <v>90</v>
       </c>
       <c r="D12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="13">
@@ -676,7 +670,7 @@
         <v>46</v>
       </c>
       <c r="D13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="14">
@@ -732,7 +726,7 @@
         <v>94</v>
       </c>
       <c r="D17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="18">
@@ -746,7 +740,7 @@
         <v>95</v>
       </c>
       <c r="D18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="19">
@@ -760,7 +754,7 @@
         <v>96</v>
       </c>
       <c r="D19" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="20">
@@ -774,7 +768,7 @@
         <v>97</v>
       </c>
       <c r="D20" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="21">
@@ -788,7 +782,7 @@
         <v>98</v>
       </c>
       <c r="D21" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="22">
@@ -802,7 +796,7 @@
         <v>99</v>
       </c>
       <c r="D22" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="23">
@@ -816,7 +810,7 @@
         <v>100</v>
       </c>
       <c r="D23" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="24">
@@ -830,7 +824,7 @@
         <v>101</v>
       </c>
       <c r="D24" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="25">
@@ -844,7 +838,7 @@
         <v>102</v>
       </c>
       <c r="D25" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="26">
@@ -858,7 +852,7 @@
         <v>103</v>
       </c>
       <c r="D26" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="27">
@@ -872,7 +866,7 @@
         <v>104</v>
       </c>
       <c r="D27" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="28">
@@ -886,7 +880,7 @@
         <v>105</v>
       </c>
       <c r="D28" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="29">
@@ -900,7 +894,7 @@
         <v>106</v>
       </c>
       <c r="D29" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="30">
@@ -914,7 +908,7 @@
         <v>107</v>
       </c>
       <c r="D30" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="31">
@@ -928,7 +922,7 @@
         <v>108</v>
       </c>
       <c r="D31" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="32">
@@ -942,7 +936,7 @@
         <v>109</v>
       </c>
       <c r="D32" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="33">
@@ -956,7 +950,7 @@
         <v>110</v>
       </c>
       <c r="D33" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="34">
@@ -970,7 +964,7 @@
         <v>111</v>
       </c>
       <c r="D34" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="35">
@@ -998,7 +992,7 @@
         <v>46</v>
       </c>
       <c r="D36" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="37">
@@ -1054,7 +1048,7 @@
         <v>115</v>
       </c>
       <c r="D40" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="41">
@@ -1079,10 +1073,10 @@
         <v>46</v>
       </c>
       <c r="C42" t="s">
-        <v>116</v>
+        <v>46</v>
       </c>
       <c r="D42" t="s">
-        <v>145</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>